<commit_message>
Avant derniere sauvegarde avant la libération
</commit_message>
<xml_diff>
--- a/TB documents/JournalTravail/Distance_Match_StopSign.xlsx
+++ b/TB documents/JournalTravail/Distance_Match_StopSign.xlsx
@@ -1,20 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c31a1cfc8e0b17/HEIG-VD/Travail de bachelor/AutonomousRcCar/JournalTravail/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/01c31a1cfc8e0b17/HEIG-VD/Travail de bachelor/AutonomousRcCar/TB documents/JournalTravail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{944B0F86-4556-48F7-8EED-4F51B6B2D500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8A891CEC-1CA3-497F-AADC-00DCB7D601A1}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{944B0F86-4556-48F7-8EED-4F51B6B2D500}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{822C42B7-D096-449D-A005-D7B34AE42EE0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{DCB6E4E1-1990-41C0-BA17-53AA369A26AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$A$2:$A$26</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$B$2:$B$26</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -115,10 +119,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -314,7 +316,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1508,7 +1509,7 @@
   <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>